<commit_message>
Added comments to test file
</commit_message>
<xml_diff>
--- a/boardLayoutTests.xlsx
+++ b/boardLayoutTests.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\adit\Desktop\ClueGame\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="18645" windowHeight="4980"/>
   </bookViews>
@@ -10,7 +15,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -520,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J32" sqref="J32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="6" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -572,7 +576,7 @@
       <c r="O1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="9" t="s">
         <v>0</v>
       </c>
       <c r="Q1" s="2" t="s">

</xml_diff>